<commit_message>
Added circuitry for testing frequency response.
</commit_message>
<xml_diff>
--- a/Mixer/Mixer Characterization.xlsx
+++ b/Mixer/Mixer Characterization.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prototype" sheetId="1" r:id="rId1"/>
+    <sheet name="Simulation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Gain (V/V)</t>
   </si>
@@ -41,13 +42,36 @@
   <si>
     <t>Maximum Output Signal at MidBand (1000Hz): 3.40Vpp</t>
   </si>
+  <si>
+    <t>3dB_H (KHz)</t>
+  </si>
+  <si>
+    <t>3dB_L (Hz)</t>
+  </si>
+  <si>
+    <t>Number of Instruments</t>
+  </si>
+  <si>
+    <t>Frequency Response For Different Number of Instruments. All wipers set to 1 on the pots.</t>
+  </si>
+  <si>
+    <t>Only one instrument is used for sweeping, rest are set to 60Hz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,14 +99,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -180,7 +225,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$D$1</c:f>
+              <c:f>Prototype!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -215,7 +260,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$36</c:f>
+              <c:f>Prototype!$A$2:$A$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -329,7 +374,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$D$2:$D$36</c:f>
+              <c:f>Prototype!$D$2:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="35"/>
@@ -1412,12 +1457,24 @@
   <tableColumns count="4">
     <tableColumn id="1" name="Signal Frequency(Hz)"/>
     <tableColumn id="5" name="Vpp"/>
-    <tableColumn id="2" name="Gain (V/V)" dataDxfId="0">
+    <tableColumn id="2" name="Gain (V/V)" dataDxfId="1">
       <calculatedColumnFormula>Table1[[#This Row],[Vpp]]/$B$18</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Gain (dB)">
       <calculatedColumnFormula>20*LOG(C2)</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C5" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:C5"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Number of Instruments"/>
+    <tableColumn id="2" name="3dB_L (Hz)"/>
+    <tableColumn id="3" name="3dB_H (KHz)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1688,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
@@ -2183,7 +2240,7 @@
         <v>0.66086956521739137</v>
       </c>
       <c r="D30">
-        <f>20*LOG(C30)</f>
+        <f t="shared" ref="D30:D36" si="1">20*LOG(C30)</f>
         <v>-3.5976849614564053</v>
       </c>
     </row>
@@ -2199,7 +2256,7 @@
         <v>0.60869565217391308</v>
       </c>
       <c r="D31">
-        <f>20*LOG(C31)</f>
+        <f t="shared" si="1"/>
         <v>-4.3119960067870968</v>
       </c>
     </row>
@@ -2215,7 +2272,7 @@
         <v>0.58695652173913049</v>
       </c>
       <c r="D32">
-        <f>20*LOG(C32)</f>
+        <f t="shared" si="1"/>
         <v>-4.6278813504517347</v>
       </c>
     </row>
@@ -2231,7 +2288,7 @@
         <v>0.56521739130434789</v>
       </c>
       <c r="D33">
-        <f>20*LOG(C33)</f>
+        <f t="shared" si="1"/>
         <v>-4.9556896742151215</v>
       </c>
     </row>
@@ -2247,7 +2304,7 @@
         <v>0.46086956521739136</v>
       </c>
       <c r="D34">
-        <f>20*LOG(C34)</f>
+        <f t="shared" si="1"/>
         <v>-6.7284394150564522</v>
       </c>
     </row>
@@ -2263,7 +2320,7 @@
         <v>0.3895652173913044</v>
       </c>
       <c r="D35">
-        <f>20*LOG(C35)</f>
+        <f t="shared" si="1"/>
         <v>-8.1883965271093526</v>
       </c>
     </row>
@@ -2279,7 +2336,7 @@
         <v>0.22782608695652176</v>
       </c>
       <c r="D36">
-        <f>20*LOG(C36)</f>
+        <f t="shared" si="1"/>
         <v>-12.847930980677324</v>
       </c>
     </row>
@@ -2291,4 +2348,112 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" activeCellId="1" sqref="B14 J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>17.38</v>
+      </c>
+      <c r="C3">
+        <v>22.9</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>17.37</v>
+      </c>
+      <c r="C4">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>17.37</v>
+      </c>
+      <c r="C5">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>17.37</v>
+      </c>
+      <c r="C6">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>17.37</v>
+      </c>
+      <c r="C7">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>